<commit_message>
planilha Game's Marvel.. relevancia feita
</commit_message>
<xml_diff>
--- a/Tweets/tweets_Game Marvel's Spider-Man - PS4_201809101603.xlsx
+++ b/Tweets/tweets_Game Marvel's Spider-Man - PS4_201809101603.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ienzo\Desktop\Insper\2° Semestre\Ciência dos Dados\Projetos\Projeto_2_CD\Tweets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709236B2-2B46-4E23-BB98-AEAFE199E8CA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5440D2AB-BC7F-4350-A7EB-2ED53699D3E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t>Treinamento</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Teste</t>
+  </si>
+  <si>
+    <t>relevancia</t>
   </si>
 </sst>
 </file>
@@ -499,245 +502,392 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A47"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>2</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correção do excel Game...
</commit_message>
<xml_diff>
--- a/Tweets/tweets_Game Marvel's Spider-Man - PS4_201809101603.xlsx
+++ b/Tweets/tweets_Game Marvel's Spider-Man - PS4_201809101603.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ienzo\Desktop\Insper\2° Semestre\Ciência dos Dados\Projetos\Projeto_2_CD\Tweets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gugat\Desktop\Insper DS 2018.1\2 semestre\Ciencia dos dados\Projeto_2_CD\Tweets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5440D2AB-BC7F-4350-A7EB-2ED53699D3E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A9332CDA-F22D-41A5-B736-887625C8FAAA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,7 +879,7 @@
         <v>20</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>